<commit_message>
updated pcb directories, sw submodule
</commit_message>
<xml_diff>
--- a/PCB/infinity_mirror_v0.9.0/BoM_v0.9.0.xlsx
+++ b/PCB/infinity_mirror_v0.9.0/BoM_v0.9.0.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="124">
   <si>
     <t>MAIN BOARD</t>
   </si>
@@ -40,7 +40,7 @@
     <t>Price/Unit</t>
   </si>
   <si>
-    <t>Total Component Price</t>
+    <t>Total Price</t>
   </si>
   <si>
     <t>Owned?</t>
@@ -170,7 +170,7 @@
     <t>CL21A106KAYNNNG</t>
   </si>
   <si>
-    <t>Power Indicator Current Limiting Resistor</t>
+    <t>Power Indicator I Limiting Resistor</t>
   </si>
   <si>
     <t>pow5</t>
@@ -254,12 +254,15 @@
     <t>0.1uF</t>
   </si>
   <si>
-    <t>Rotary Encoder w/ 12 Detents + button</t>
+    <t>Rotary Encoder w/ button</t>
   </si>
   <si>
     <t>enc2</t>
   </si>
   <si>
+    <t>12 detents</t>
+  </si>
+  <si>
     <t>NA</t>
   </si>
   <si>
@@ -329,9 +332,6 @@
     <t>Total Components</t>
   </si>
   <si>
-    <t>Total Price</t>
-  </si>
-  <si>
     <t>EXTERNAL</t>
   </si>
   <si>
@@ -348,6 +348,18 @@
   </si>
   <si>
     <t>T6634ST</t>
+  </si>
+  <si>
+    <t>WS2812b LED Strip</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <t>Mirror</t>
   </si>
   <si>
     <t>USB to UART Bridge</t>
@@ -381,7 +393,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -443,6 +455,10 @@
     <font>
       <u/>
       <color rgb="FF1155CC"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -599,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="81">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -785,6 +801,21 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -794,7 +825,7 @@
     <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -809,13 +840,13 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1034,17 +1065,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.88"/>
+    <col customWidth="1" min="1" max="1" width="27.88"/>
     <col customWidth="1" min="2" max="3" width="18.88"/>
     <col customWidth="1" min="4" max="4" width="22.38"/>
-    <col customWidth="1" min="5" max="5" width="8.0"/>
+    <col customWidth="1" min="5" max="5" width="6.13"/>
     <col customWidth="1" min="6" max="6" width="12.38"/>
     <col customWidth="1" min="7" max="7" width="21.38"/>
     <col customWidth="1" min="8" max="8" width="13.38"/>
-    <col customWidth="1" min="9" max="9" width="27.25"/>
-    <col customWidth="1" min="10" max="10" width="12.63"/>
-    <col customWidth="1" min="12" max="12" width="14.0"/>
-    <col customWidth="1" min="13" max="13" width="31.38"/>
+    <col customWidth="1" min="9" max="9" width="10.88"/>
+    <col customWidth="1" min="10" max="11" width="12.63"/>
+    <col customWidth="1" min="12" max="12" width="12.0"/>
+    <col customWidth="1" min="13" max="13" width="31.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1778,9 +1809,11 @@
       <c r="B23" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="21"/>
+      <c r="C23" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="D23" s="21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E23" s="21">
         <v>1.0</v>
@@ -1789,7 +1822,7 @@
         <v>17</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H23" s="15">
         <v>2.16</v>
@@ -1809,10 +1842,10 @@
     </row>
     <row r="24">
       <c r="A24" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>72</v>
@@ -1827,7 +1860,7 @@
         <v>17</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H24" s="15">
         <v>0.1</v>
@@ -1847,14 +1880,14 @@
     </row>
     <row r="25">
       <c r="A25" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E25" s="21">
         <v>1.0</v>
@@ -1863,7 +1896,7 @@
         <v>17</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H25" s="15">
         <v>1.5</v>
@@ -1883,7 +1916,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1900,13 +1933,13 @@
     </row>
     <row r="27">
       <c r="A27" s="54" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27" s="55"/>
       <c r="E27" s="21">
@@ -1916,7 +1949,7 @@
         <v>17</v>
       </c>
       <c r="G27" s="55" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H27" s="15">
         <v>0.95</v>
@@ -1936,13 +1969,13 @@
     </row>
     <row r="28">
       <c r="A28" s="20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D28" s="21">
         <v>805.0</v>
@@ -1974,16 +2007,16 @@
     </row>
     <row r="29">
       <c r="A29" s="28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E29" s="29">
         <v>1.0</v>
@@ -1992,7 +2025,7 @@
         <v>17</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H29" s="29">
         <v>0.1</v>
@@ -2012,14 +2045,14 @@
     </row>
     <row r="30">
       <c r="D30" s="58" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E30" s="59">
         <f>SUM(E4:E29)</f>
         <v>32</v>
       </c>
       <c r="H30" s="60" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="I30" s="61">
         <f>SUM(I1:I29)</f>
@@ -2049,7 +2082,7 @@
       <c r="M32" s="10"/>
     </row>
     <row r="33">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="50" t="s">
         <v>107</v>
       </c>
       <c r="B33" s="21" t="s">
@@ -2058,7 +2091,7 @@
       <c r="C33" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="21" t="s">
         <v>110</v>
       </c>
       <c r="E33" s="21">
@@ -2087,100 +2120,108 @@
       <c r="B34" s="66"/>
       <c r="C34" s="66"/>
       <c r="D34" s="66"/>
-      <c r="E34" s="67">
+      <c r="E34" s="66">
         <v>1.0</v>
       </c>
-      <c r="F34" s="68" t="s">
+      <c r="F34" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" s="68"/>
+      <c r="H34" s="66">
+        <v>24.95</v>
+      </c>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="66"/>
+      <c r="J36" s="66"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="72">
+        <v>1.0</v>
+      </c>
+      <c r="F37" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="H34" s="66"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="67" t="s">
+      <c r="G37" s="73" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" s="71"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="K34" s="69"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="71" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="10"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="72" t="s">
-        <v>116</v>
-      </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" s="25">
+      <c r="K37" s="74"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="64"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="64"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="10"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="25">
         <v>2.0</v>
       </c>
-      <c r="F37" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="72" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-    </row>
-    <row r="39">
-      <c r="B39" s="45"/>
-      <c r="C39" s="74"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-    </row>
-    <row r="40">
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
+      <c r="F40" s="78" t="s">
+        <v>122</v>
+      </c>
       <c r="G40" s="45"/>
       <c r="H40" s="45"/>
       <c r="I40" s="45"/>
@@ -2188,11 +2229,16 @@
       <c r="K40" s="45"/>
     </row>
     <row r="41">
+      <c r="A41" s="77" t="s">
+        <v>123</v>
+      </c>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
-      <c r="D41" s="45"/>
+      <c r="D41" s="25"/>
       <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
+      <c r="F41" s="78" t="s">
+        <v>122</v>
+      </c>
       <c r="G41" s="45"/>
       <c r="H41" s="45"/>
       <c r="I41" s="45"/>
@@ -2201,10 +2247,9 @@
     </row>
     <row r="42">
       <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
+      <c r="C42" s="79"/>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
       <c r="G42" s="45"/>
       <c r="H42" s="45"/>
       <c r="I42" s="45"/>
@@ -2212,10 +2257,30 @@
       <c r="K42" s="45"/>
     </row>
     <row r="43">
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
       <c r="K43" s="45"/>
     </row>
+    <row r="44">
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="45"/>
+    </row>
     <row r="45">
-      <c r="A45" s="75"/>
       <c r="B45" s="45"/>
       <c r="C45" s="45"/>
       <c r="D45" s="45"/>
@@ -2228,49 +2293,65 @@
       <c r="K45" s="45"/>
     </row>
     <row r="46">
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
       <c r="K46" s="45"/>
     </row>
-    <row r="47">
-      <c r="A47" s="75"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="K47" s="45"/>
-    </row>
     <row r="48">
-      <c r="A48" s="75"/>
-      <c r="D48" s="25"/>
+      <c r="A48" s="80"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="45"/>
     </row>
     <row r="49">
-      <c r="A49" s="75"/>
-      <c r="D49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="K49" s="45"/>
     </row>
     <row r="50">
-      <c r="A50" s="75"/>
+      <c r="A50" s="80"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
       <c r="D50" s="25"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="K50" s="45"/>
     </row>
     <row r="51">
-      <c r="A51" s="75"/>
+      <c r="A51" s="80"/>
       <c r="D51" s="25"/>
     </row>
     <row r="52">
+      <c r="A52" s="80"/>
       <c r="D52" s="25"/>
     </row>
     <row r="53">
-      <c r="A53" s="75"/>
+      <c r="A53" s="80"/>
+      <c r="D53" s="25"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="80"/>
+      <c r="D54" s="25"/>
+    </row>
+    <row r="55">
+      <c r="D55" s="25"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="80"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2298,10 +2379,11 @@
     <hyperlink r:id="rId22" ref="F29"/>
     <hyperlink r:id="rId23" ref="F33"/>
     <hyperlink r:id="rId24" ref="F34"/>
-    <hyperlink r:id="rId25" ref="G34"/>
-    <hyperlink r:id="rId26" ref="F37"/>
-    <hyperlink r:id="rId27" ref="F38"/>
+    <hyperlink r:id="rId25" ref="F37"/>
+    <hyperlink r:id="rId26" ref="G37"/>
+    <hyperlink r:id="rId27" ref="F40"/>
+    <hyperlink r:id="rId28" ref="F41"/>
   </hyperlinks>
-  <drawing r:id="rId28"/>
+  <drawing r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>